<commit_message>
changes, in readme, etl.py and invoice.py, as well as dockerfile, requirements
</commit_message>
<xml_diff>
--- a/Elevators.xlsx
+++ b/Elevators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Desktop/Invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0BE6DD-E82D-CD43-816A-C1AFC08373C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60CEF6-2304-D142-AC47-2D63684B6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsRules" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="244">
   <si>
     <t>part_id</t>
   </si>
@@ -140,15 +140,9 @@
     <t>AKIS-VF3X 9KW</t>
   </si>
   <si>
-    <t>MOTOR 0.71M/S 990KG DOBLE TAMBOR 400*10</t>
-  </si>
-  <si>
     <t>AKIS-ZF603KW/DT</t>
   </si>
   <si>
-    <t>MOTOR DOBLE TAMBOR 0.46M/S 250KG</t>
-  </si>
-  <si>
     <t>AKIS-ZF604KW</t>
   </si>
   <si>
@@ -407,24 +401,6 @@
     <t>CABLE  VIAJERO 24 HILOS</t>
   </si>
   <si>
-    <t>ELEASC260</t>
-  </si>
-  <si>
-    <t>DISPLAY NICE 1000</t>
-  </si>
-  <si>
-    <t>ELEASC281</t>
-  </si>
-  <si>
-    <t>DISPLAY MCTC-HCB-R1</t>
-  </si>
-  <si>
-    <t>ELEASC282</t>
-  </si>
-  <si>
-    <t>DISPLAY MCTC-HCB-U1</t>
-  </si>
-  <si>
     <t>ESBASC028</t>
   </si>
   <si>
@@ -542,18 +518,9 @@
     <t>NICE-CBI-B-4007</t>
   </si>
   <si>
-    <t>CONTROL MONARCH DE CABINA  5.5KW 220V  NICE L-C-4007</t>
-  </si>
-  <si>
     <t>NICE-CBI-B-F15</t>
   </si>
   <si>
-    <t>CONTROL MONARCH DE CABINA  7.5KW 3 FASES 220V  NICE L-C-4015</t>
-  </si>
-  <si>
-    <t>CONTROL MONARCH DE CABINA  11KW 3 FASES 220V  NICE L-C-4018</t>
-  </si>
-  <si>
     <t>ON-01 LIFT CAM</t>
   </si>
   <si>
@@ -662,15 +629,6 @@
     <t xml:space="preserve">acces_control </t>
   </si>
   <si>
-    <t>ceil(0.6*F)</t>
-  </si>
-  <si>
-    <t>gearless</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>ceil(6*F)</t>
   </si>
   <si>
@@ -753,13 +711,70 @@
   </si>
   <si>
     <t>F&gt;=3 and door_type=="manuales"</t>
+  </si>
+  <si>
+    <t>por piso mas el cuarto de maquibas</t>
+  </si>
+  <si>
+    <t>MOTOR 0.71M/S 990KG DOBLE TAMBOR 400*10 no buufer plasrtico</t>
+  </si>
+  <si>
+    <t>MOTOR DOBLE TAMBOR 0.46M/S 250KG no buffer plastico</t>
+  </si>
+  <si>
+    <t>CONTROL MONARCH DE CABINA  11KW 3 FASES 220V  NICE L-C-4018 - 3000</t>
+  </si>
+  <si>
+    <t>CONTROL MONARCH DE CABINA  7.5KW 3 FASES 220V  NICE L-C-4015 - 3000</t>
+  </si>
+  <si>
+    <t>CONTROL MONARCH DE CABINA  5.5KW 220V  NICE L-C-4007 - 3000</t>
+  </si>
+  <si>
+    <t>PARTE LECTRICA</t>
+  </si>
+  <si>
+    <t>ELE</t>
+  </si>
+  <si>
+    <t>ASC131</t>
+  </si>
+  <si>
+    <t>CABLE DE ACERO # 8 MM</t>
+  </si>
+  <si>
+    <t>3*F</t>
+  </si>
+  <si>
+    <t>2 if machine_room and not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 3</t>
+  </si>
+  <si>
+    <t>ceil(0.6 * F) if (not machine_room and not hydraulic_cylinder and ((12 &lt; P &lt; 14) or (13 &lt; P &lt;= 16))) else 0</t>
+  </si>
+  <si>
+    <t>2 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 10</t>
+  </si>
+  <si>
+    <t>ceil(1.4 * F) if (not hydraulic_cylinder and (P &lt;= 3 or (6 &lt; P &lt; 10))) else 0</t>
+  </si>
+  <si>
+    <t>2 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 4</t>
+  </si>
+  <si>
+    <t>0 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 if (not hydraulic_cylinder and (P &lt;= 3 or (6 &lt; P &lt; 10))) else ceil(1.4 * F) </t>
+  </si>
+  <si>
+    <t>0 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,6 +816,11 @@
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -845,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -860,9 +880,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,13 +1218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B74E1E-2FAB-A84A-BD4C-ED601BD34DA2}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="101.1640625" customWidth="1"/>
@@ -1215,7 +1236,7 @@
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,16 +1256,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1262,19 +1283,19 @@
         <v>3475.5529999999994</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1292,19 +1313,19 @@
         <v>3679.9999999999995</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1322,19 +1343,19 @@
         <v>2964.4470000000001</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1352,19 +1373,19 @@
         <v>3577.7764999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1382,19 +1403,19 @@
         <v>3085.1279999999997</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1412,24 +1433,24 @@
         <v>3986.6704999999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="C8" s="1">
         <v>2534.1733330000002</v>
@@ -1442,24 +1463,24 @@
         <v>4499.9959999999992</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>1036.77</v>
@@ -1472,24 +1493,24 @@
         <v>2351.1174999999998</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>233</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1">
         <v>1043.123333</v>
@@ -1502,24 +1523,24 @@
         <v>2300</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>1157.7049999999999</v>
@@ -1532,24 +1553,24 @@
         <v>2875</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C12" s="1">
         <v>1115.56</v>
@@ -1562,24 +1583,24 @@
         <v>2530</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C13" s="1">
         <v>1046.06</v>
@@ -1592,24 +1613,24 @@
         <v>2875</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C14" s="1">
         <v>1154.93</v>
@@ -1622,24 +1643,24 @@
         <v>2633.6609999999996</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1">
         <v>1170.92</v>
@@ -1652,22 +1673,22 @@
         <v>1856.2839999999999</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C16" s="1">
         <v>1444.15</v>
@@ -1680,22 +1701,22 @@
         <v>2134.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="C17" s="1">
         <v>1170.92</v>
@@ -1708,20 +1729,20 @@
         <v>2231</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="C18" s="1">
         <v>963.69500000000005</v>
@@ -1734,20 +1755,20 @@
         <v>3300.0054999999998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="C19" s="1">
         <v>1163.49</v>
@@ -1760,20 +1781,20 @@
         <v>3399.9979999999996</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C20" s="1">
         <v>290</v>
@@ -1792,16 +1813,16 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C21" s="1">
         <v>201.5</v>
@@ -1817,17 +1838,17 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C22" s="1">
         <v>69.69</v>
@@ -1843,17 +1864,17 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C23" s="1">
         <v>21.476064999999998</v>
@@ -1869,43 +1890,43 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" s="8">
+        <v>169</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="1">
         <v>61.337499999999999</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="1">
         <v>252.17</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="1">
         <f t="shared" ref="E24" si="3">+D24*1.15</f>
         <v>289.99549999999994</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="1">
         <v>3</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="H24" s="12"/>
+      <c r="G24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C25" s="1">
         <v>36.6</v>
@@ -1921,19 +1942,19 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C26" s="1">
         <v>109</v>
@@ -1949,19 +1970,19 @@
         <v>3</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C27" s="1">
         <v>24.002386000000001</v>
@@ -1974,22 +1995,19 @@
         <v>78.602499999999992</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="G27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1">
         <v>182.813333</v>
@@ -2005,17 +2023,17 @@
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1">
         <v>533.625</v>
@@ -2031,17 +2049,17 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30" s="1">
         <v>99.29</v>
@@ -2057,17 +2075,17 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1">
         <v>126.91249999999999</v>
@@ -2083,12 +2101,12 @@
         <v>2</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -2114,7 +2132,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -2140,7 +2158,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2166,7 +2184,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -2192,7 +2210,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -2218,7 +2236,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -2244,7 +2262,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -2270,12 +2288,12 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1">
         <v>2.2000000000000002</v>
@@ -2296,12 +2314,12 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1">
         <v>2.5</v>
@@ -2322,12 +2340,12 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1">
         <v>15.8</v>
@@ -2348,12 +2366,12 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1">
         <v>135.4</v>
@@ -2374,12 +2392,12 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1">
         <v>50</v>
@@ -2400,12 +2418,12 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1">
         <v>26.9</v>
@@ -2426,12 +2444,12 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C45" s="1">
         <v>6.1</v>
@@ -2452,12 +2470,12 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C46" s="1">
         <v>1.4999999999999999E-2</v>
@@ -2470,7 +2488,7 @@
         <v>1.5984999999999998</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>1</v>
@@ -2478,12 +2496,12 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C47" s="1">
         <v>19</v>
@@ -2504,12 +2522,12 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C48" s="1">
         <v>19.096</v>
@@ -2518,7 +2536,7 @@
         <v>5.82</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" ref="E48:E57" si="7">+D48*1.15</f>
+        <f t="shared" ref="E48:E58" si="7">+D48*1.15</f>
         <v>6.6929999999999996</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -2530,12 +2548,12 @@
       <c r="H48" s="3"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" s="1">
         <v>13.708636</v>
@@ -2556,12 +2574,12 @@
       <c r="H49" s="3"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" s="1">
         <v>500</v>
@@ -2582,12 +2600,12 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C51" s="1">
         <v>2.99</v>
@@ -2608,129 +2626,129 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="1">
+    <row r="52" spans="1:9">
+      <c r="A52" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="D52" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="E52" s="8">
+        <f t="shared" si="7"/>
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="8">
         <v>2.27</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="12">
         <v>4.1900000000000004</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E53" s="8">
         <f t="shared" si="7"/>
         <v>4.8185000000000002</v>
       </c>
-      <c r="F52" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="F53" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="1">
         <v>157.99333300000001</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <v>401.79</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E54" s="1">
         <f t="shared" si="7"/>
         <v>462.05849999999998</v>
       </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="1">
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="1">
         <v>13.108750000000001</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <v>53.57</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E55" s="1">
         <f t="shared" si="7"/>
         <v>61.605499999999992</v>
       </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-      <c r="G54" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="1">
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="1">
         <v>56.094999999999999</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <v>98.57</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E56" s="1">
         <f t="shared" si="7"/>
         <v>113.35549999999998</v>
       </c>
-      <c r="F55" s="1">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="1">
-        <v>35.036999999999999</v>
-      </c>
-      <c r="D56" s="4">
-        <v>73.930000000000007</v>
-      </c>
-      <c r="E56" s="1">
-        <f t="shared" si="7"/>
-        <v>85.019500000000008</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>2</v>
+      <c r="F56" s="1">
+        <v>1</v>
       </c>
       <c r="G56" s="1" t="b">
         <v>1</v>
@@ -2738,25 +2756,25 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1">
-        <v>2.3317999999999999</v>
+        <v>45.5</v>
       </c>
       <c r="D57" s="4">
-        <v>7.83</v>
+        <v>100</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="7"/>
-        <v>9.0045000000000002</v>
-      </c>
-      <c r="F57" s="1">
-        <v>6</v>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="G57" s="1" t="b">
         <v>1</v>
@@ -2764,24 +2782,25 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58" s="7">
-        <v>11.78</v>
-      </c>
-      <c r="D58" s="5">
-        <v>10.84</v>
-      </c>
-      <c r="E58" s="7">
-        <v>12.463240000000001</v>
-      </c>
-      <c r="F58" s="7">
-        <v>4</v>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2.3317999999999999</v>
+      </c>
+      <c r="D58" s="4">
+        <v>7.83</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="7"/>
+        <v>9.0045000000000002</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6</v>
       </c>
       <c r="G58" s="1" t="b">
         <v>1</v>
@@ -2789,25 +2808,24 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="1">
-        <v>427</v>
-      </c>
-      <c r="D59" s="4">
-        <v>736</v>
-      </c>
-      <c r="E59" s="1">
-        <f t="shared" ref="E59:E64" si="8">+D59*1.15</f>
-        <v>846.4</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1</v>
+    <row r="59" spans="1:9">
+      <c r="A59" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="7">
+        <v>11.78</v>
+      </c>
+      <c r="D59" s="5">
+        <v>10.84</v>
+      </c>
+      <c r="E59" s="7">
+        <v>12.463240000000001</v>
+      </c>
+      <c r="F59" s="7">
+        <v>4</v>
       </c>
       <c r="G59" s="1" t="b">
         <v>1</v>
@@ -2815,103 +2833,103 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C60" s="1">
+        <v>427</v>
+      </c>
+      <c r="D60" s="4">
+        <v>736</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" ref="E60:E65" si="8">+D60*1.15</f>
+        <v>846.4</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="1">
         <v>14.5</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <v>40.869999999999997</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E61" s="1">
         <f t="shared" si="8"/>
         <v>47.000499999999995</v>
       </c>
-      <c r="F60" s="1">
-        <v>1</v>
-      </c>
-      <c r="G60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="1">
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="1">
         <v>1.6983000000000002E-2</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <v>2.23</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E62" s="1">
         <f t="shared" si="8"/>
         <v>2.5644999999999998</v>
       </c>
-      <c r="F61" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="G61" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="1">
+      <c r="F62" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="G62" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="1">
         <v>1.159999</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <v>16.43</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <f t="shared" si="8"/>
         <v>18.894499999999997</v>
       </c>
-      <c r="F62" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G62" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C63" s="1">
-        <v>5</v>
-      </c>
-      <c r="D63" s="4">
-        <v>7.36</v>
-      </c>
-      <c r="E63" s="1">
-        <f t="shared" si="8"/>
-        <v>8.4640000000000004</v>
-      </c>
       <c r="F63" s="7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G63" s="1" t="b">
         <v>1</v>
@@ -2919,12 +2937,12 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C64" s="1">
         <v>5</v>
@@ -2937,7 +2955,7 @@
         <v>8.4640000000000004</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="G64" s="1" t="b">
         <v>1</v>
@@ -2945,235 +2963,235 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+    <row r="65" spans="1:9">
+      <c r="A65" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="1">
+        <v>5</v>
+      </c>
+      <c r="D65" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="8"/>
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G65" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="1">
+        <v>975</v>
+      </c>
+      <c r="D66" s="4">
+        <v>1794</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" ref="E66:E82" si="9">+D66*1.15</f>
+        <v>2063.1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B67" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="8">
-        <v>975</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1794</v>
-      </c>
-      <c r="E65" s="8">
-        <f t="shared" ref="E65:E84" si="9">+D65*1.15</f>
-        <v>2063.1</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C66" s="1">
+      <c r="C67" s="1">
         <v>15.65</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <v>35.71</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E67" s="1">
         <f t="shared" si="9"/>
         <v>41.066499999999998</v>
       </c>
-      <c r="F66" s="1">
-        <v>1</v>
-      </c>
-      <c r="G66" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="1">
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="1">
         <v>11.55</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <v>12.24</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E68" s="1">
         <f t="shared" si="9"/>
         <v>14.075999999999999</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F68" s="1">
         <v>2</v>
       </c>
-      <c r="G67" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="1">
+      <c r="G68" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69" s="1">
         <v>3.38</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <v>3.68</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E69" s="1">
         <f t="shared" si="9"/>
         <v>4.2320000000000002</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F69" s="1">
         <v>3</v>
       </c>
-      <c r="G68" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="G69" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="1">
         <v>5.26</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <v>6.44</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E70" s="1">
         <f t="shared" si="9"/>
         <v>7.4059999999999997</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F70" s="7">
         <v>0.25</v>
       </c>
-      <c r="G69" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C70" s="1">
+      <c r="G70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="1">
         <v>18.78</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <v>45.18</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E71" s="1">
         <f t="shared" si="9"/>
         <v>51.956999999999994</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G70" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C71" s="1">
+      <c r="G71" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="1">
         <v>138</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <v>164.31</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E72" s="1">
         <f t="shared" si="9"/>
         <v>188.95649999999998</v>
       </c>
-      <c r="F71" s="1">
-        <v>1</v>
-      </c>
-      <c r="G71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C72" s="1">
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="1">
         <v>3.6944720000000002</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <v>8.52</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E73" s="1">
         <f t="shared" si="9"/>
         <v>9.7979999999999983</v>
       </c>
-      <c r="F72" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="G72" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C73" s="1">
-        <v>15</v>
-      </c>
-      <c r="D73" s="4">
-        <v>50</v>
-      </c>
-      <c r="E73" s="1">
-        <f t="shared" si="9"/>
-        <v>57.499999999999993</v>
-      </c>
       <c r="F73" s="7" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="G73" s="1" t="b">
         <v>1</v>
@@ -3181,51 +3199,51 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="1">
-        <v>12.926667</v>
-      </c>
-      <c r="D74" s="4">
-        <v>49.57</v>
-      </c>
-      <c r="E74" s="1">
+    <row r="74" spans="1:9">
+      <c r="A74" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="8">
+        <v>7.25</v>
+      </c>
+      <c r="D74" s="12">
+        <v>31.25</v>
+      </c>
+      <c r="E74" s="8">
         <f t="shared" si="9"/>
-        <v>57.005499999999998</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G74" s="1" t="b">
+        <v>35.9375</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="G74" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C75" s="1">
-        <v>25</v>
+        <v>31.195667</v>
       </c>
       <c r="D75" s="4">
-        <v>62.5</v>
+        <v>84.82</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" si="9"/>
-        <v>71.875</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>2</v>
+        <v>97.542999999999978</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1</v>
       </c>
       <c r="G75" s="1" t="b">
         <v>1</v>
@@ -3233,22 +3251,22 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C76" s="1">
-        <v>7.25</v>
+        <v>100.704865</v>
       </c>
       <c r="D76" s="4">
-        <v>31.25</v>
+        <v>321.74</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" si="9"/>
-        <v>35.9375</v>
+        <v>370.00099999999998</v>
       </c>
       <c r="F76" s="1">
         <v>1</v>
@@ -3259,22 +3277,22 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C77" s="1">
-        <v>31.195667</v>
+        <v>82.356999999999999</v>
       </c>
       <c r="D77" s="4">
-        <v>84.82</v>
+        <v>357.14</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" si="9"/>
-        <v>97.542999999999978</v>
+        <v>410.71099999999996</v>
       </c>
       <c r="F77" s="1">
         <v>1</v>
@@ -3285,67 +3303,67 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C78" s="1">
-        <v>100.704865</v>
-      </c>
-      <c r="D78" s="4">
-        <v>321.74</v>
-      </c>
-      <c r="E78" s="1">
+    <row r="78" spans="1:9">
+      <c r="A78" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C78" s="8">
+        <v>3.872404</v>
+      </c>
+      <c r="D78" s="12">
+        <v>16.07</v>
+      </c>
+      <c r="E78" s="8">
         <f t="shared" si="9"/>
-        <v>370.00099999999998</v>
-      </c>
-      <c r="F78" s="1">
-        <v>1</v>
-      </c>
-      <c r="G78" s="1" t="b">
+        <v>18.480499999999999</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G78" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="1">
-        <v>82.356999999999999</v>
-      </c>
-      <c r="D79" s="4">
-        <v>357.14</v>
-      </c>
-      <c r="E79" s="1">
+    <row r="79" spans="1:9">
+      <c r="A79" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="8">
+        <v>16.879968999999999</v>
+      </c>
+      <c r="D79" s="12">
+        <v>19.57</v>
+      </c>
+      <c r="E79" s="8">
         <f t="shared" si="9"/>
-        <v>410.71099999999996</v>
-      </c>
-      <c r="F79" s="1">
-        <v>1</v>
-      </c>
-      <c r="G79" s="1" t="b">
+        <v>22.505499999999998</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G79" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C80" s="1">
-        <v>3.872404</v>
+        <v>6.7</v>
       </c>
       <c r="D80" s="4">
         <v>16.07</v>
@@ -3354,8 +3372,8 @@
         <f t="shared" si="9"/>
         <v>18.480499999999999</v>
       </c>
-      <c r="F80" s="1">
-        <v>10</v>
+      <c r="F80" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="G80" s="1" t="b">
         <v>1</v>
@@ -3363,25 +3381,25 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C81" s="1">
-        <v>16.879968999999999</v>
+        <v>36.583019</v>
       </c>
       <c r="D81" s="4">
-        <v>19.57</v>
+        <v>104.35</v>
       </c>
       <c r="E81" s="1">
         <f t="shared" si="9"/>
-        <v>22.505499999999998</v>
-      </c>
-      <c r="F81" s="1">
-        <v>10</v>
+        <v>120.00249999999998</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="G81" s="1" t="b">
         <v>1</v>
@@ -3389,51 +3407,50 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C82" s="1">
-        <v>6.7</v>
-      </c>
-      <c r="D82" s="4">
-        <v>16.07</v>
-      </c>
-      <c r="E82" s="1">
+    <row r="82" spans="1:9">
+      <c r="A82" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" s="8">
+        <v>56.479194999999997</v>
+      </c>
+      <c r="D82" s="12">
+        <v>140.18</v>
+      </c>
+      <c r="E82" s="8">
         <f t="shared" si="9"/>
-        <v>18.480499999999999</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G82" s="1" t="b">
+        <v>161.20699999999999</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="G82" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C83" s="1">
-        <v>36.583019</v>
+        <v>300</v>
       </c>
       <c r="D83" s="4">
-        <v>104.35</v>
+        <v>300</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="9"/>
-        <v>120.00249999999998</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>208</v>
+        <v>300</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="G83" s="1" t="b">
         <v>1</v>
@@ -3441,25 +3458,25 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C84" s="1">
-        <v>56.479194999999997</v>
+        <v>240.5</v>
       </c>
       <c r="D84" s="4">
-        <v>140.18</v>
+        <v>358.8</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="9"/>
-        <v>161.20699999999999</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>208</v>
+        <f t="shared" ref="E84:E96" si="10">+D84*1.15</f>
+        <v>412.62</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
       </c>
       <c r="G84" s="1" t="b">
         <v>1</v>
@@ -3467,24 +3484,25 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C85" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="D85" s="4">
-        <v>300</v>
+        <v>112.32</v>
       </c>
       <c r="E85" s="1">
-        <v>300</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>129.16799999999998</v>
+      </c>
+      <c r="F85" s="1">
+        <v>1</v>
       </c>
       <c r="G85" s="1" t="b">
         <v>1</v>
@@ -3492,25 +3510,25 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C86" s="1">
-        <v>240.5</v>
+        <v>4</v>
       </c>
       <c r="D86" s="4">
-        <v>358.8</v>
+        <v>16</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" ref="E86:E97" si="10">+D86*1.15</f>
-        <v>412.62</v>
+        <f t="shared" si="10"/>
+        <v>18.399999999999999</v>
       </c>
       <c r="F86" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G86" s="1" t="b">
         <v>1</v>
@@ -3518,25 +3536,25 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C87" s="1">
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="D87" s="4">
-        <v>112.32</v>
+        <v>16.559999999999999</v>
       </c>
       <c r="E87" s="1">
         <f t="shared" si="10"/>
-        <v>129.16799999999998</v>
+        <v>19.043999999999997</v>
       </c>
       <c r="F87" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G87" s="1" t="b">
         <v>1</v>
@@ -3544,22 +3562,22 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C88" s="1">
-        <v>4</v>
+        <v>5.89</v>
       </c>
       <c r="D88" s="4">
-        <v>16</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="E88" s="1">
         <f t="shared" si="10"/>
-        <v>18.399999999999999</v>
+        <v>9.5219999999999985</v>
       </c>
       <c r="F88" s="1">
         <v>2</v>
@@ -3570,25 +3588,25 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C89" s="1">
-        <v>13.5</v>
+        <v>60</v>
       </c>
       <c r="D89" s="4">
-        <v>16.559999999999999</v>
+        <v>134.78</v>
       </c>
       <c r="E89" s="1">
         <f t="shared" si="10"/>
-        <v>19.043999999999997</v>
+        <v>154.99699999999999</v>
       </c>
       <c r="F89" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G89" s="1" t="b">
         <v>1</v>
@@ -3596,25 +3614,25 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C90" s="1">
-        <v>5.89</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="D90" s="4">
-        <v>8.2799999999999994</v>
+        <v>21.74</v>
       </c>
       <c r="E90" s="1">
         <f t="shared" si="10"/>
-        <v>9.5219999999999985</v>
+        <v>25.000999999999998</v>
       </c>
       <c r="F90" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G90" s="1" t="b">
         <v>1</v>
@@ -3622,25 +3640,25 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C91" s="1">
-        <v>60</v>
-      </c>
-      <c r="D91" s="4">
-        <v>134.78</v>
-      </c>
-      <c r="E91" s="1">
+    <row r="91" spans="1:9">
+      <c r="A91" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" s="8">
+        <v>3.55</v>
+      </c>
+      <c r="D91" s="12">
+        <v>8.48</v>
+      </c>
+      <c r="E91" s="8">
         <f t="shared" si="10"/>
-        <v>154.99699999999999</v>
-      </c>
-      <c r="F91" s="1">
-        <v>1</v>
+        <v>9.7519999999999989</v>
+      </c>
+      <c r="F91" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="G91" s="1" t="b">
         <v>1</v>
@@ -3648,25 +3666,25 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C92" s="1">
-        <v>8.7100000000000009</v>
-      </c>
-      <c r="D92" s="4">
-        <v>21.74</v>
-      </c>
-      <c r="E92" s="1">
+    <row r="92" spans="1:9">
+      <c r="A92" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="8">
+        <v>61.337499999999999</v>
+      </c>
+      <c r="D92" s="12">
+        <v>252.17</v>
+      </c>
+      <c r="E92" s="8">
         <f t="shared" si="10"/>
-        <v>25.000999999999998</v>
-      </c>
-      <c r="F92" s="1">
-        <v>4</v>
+        <v>289.99549999999994</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>236</v>
       </c>
       <c r="G92" s="1" t="b">
         <v>1</v>
@@ -3674,25 +3692,25 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C93" s="1">
-        <v>3.55</v>
-      </c>
-      <c r="D93" s="4">
-        <v>8.48</v>
-      </c>
-      <c r="E93" s="1">
+    <row r="93" spans="1:9">
+      <c r="A93" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C93" s="8">
+        <v>80</v>
+      </c>
+      <c r="D93" s="12">
+        <v>80</v>
+      </c>
+      <c r="E93" s="8">
         <f t="shared" si="10"/>
-        <v>9.7519999999999989</v>
-      </c>
-      <c r="F93" s="1">
-        <v>4</v>
+        <v>92</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="G93" s="1" t="b">
         <v>1</v>
@@ -3700,25 +3718,25 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C94" s="1">
-        <v>61.337499999999999</v>
+        <v>3.5</v>
       </c>
       <c r="D94" s="4">
-        <v>252.17</v>
+        <v>6</v>
       </c>
       <c r="E94" s="1">
         <f t="shared" si="10"/>
-        <v>289.99549999999994</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="F94" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G94" s="1" t="b">
         <v>1</v>
@@ -3726,25 +3744,25 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="C95" s="1">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="D95" s="4">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E95" s="1">
         <f t="shared" si="10"/>
-        <v>92</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>210</v>
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="F95" s="1">
+        <v>1</v>
       </c>
       <c r="G95" s="1" t="b">
         <v>1</v>
@@ -3752,57 +3770,36 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C96" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="D96" s="4">
-        <v>6</v>
-      </c>
-      <c r="E96" s="1">
+    <row r="96" spans="1:9">
+      <c r="A96" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C96" s="8">
+        <v>800</v>
+      </c>
+      <c r="D96" s="12">
+        <v>1500</v>
+      </c>
+      <c r="E96" s="8">
         <f t="shared" si="10"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="F96" s="1">
-        <v>1</v>
-      </c>
-      <c r="G96" s="1" t="b">
+        <v>1724.9999999999998</v>
+      </c>
+      <c r="F96" s="8">
+        <v>1</v>
+      </c>
+      <c r="G96" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C97" s="1">
-        <v>6</v>
-      </c>
-      <c r="D97" s="4">
-        <v>6</v>
-      </c>
-      <c r="E97" s="1">
-        <f t="shared" si="10"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="F97" s="1">
-        <v>1</v>
-      </c>
-      <c r="G97" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
+    <row r="100" spans="2:2">
+      <c r="B100" t="s">
+        <v>225</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
changes in word doc added a new one and requirements.txt
</commit_message>
<xml_diff>
--- a/Elevators.xlsx
+++ b/Elevators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Desktop/Invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60CEF6-2304-D142-AC47-2D63684B6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD35D49-254F-A34C-B6D3-3D3AEE60791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="24140" windowHeight="17820" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsRules" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="242">
   <si>
     <t>part_id</t>
   </si>
@@ -435,12 +435,6 @@
   </si>
   <si>
     <t>TEMPLADORES M10</t>
-  </si>
-  <si>
-    <t>FEASC015</t>
-  </si>
-  <si>
-    <t>TEMPLADORES M6</t>
   </si>
   <si>
     <t>FEASC022</t>
@@ -865,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -882,8 +876,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B74E1E-2FAB-A84A-BD4C-ED601BD34DA2}">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1256,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1283,16 +1279,16 @@
         <v>3475.5529999999994</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1313,16 +1309,16 @@
         <v>3679.9999999999995</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1343,16 +1339,16 @@
         <v>2964.4470000000001</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1373,16 +1369,16 @@
         <v>3577.7764999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1403,16 +1399,16 @@
         <v>3085.1279999999997</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1433,16 +1429,16 @@
         <v>3986.6704999999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1450,7 +1446,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C8" s="1">
         <v>2534.1733330000002</v>
@@ -1463,16 +1459,16 @@
         <v>4499.9959999999992</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1480,7 +1476,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C9" s="1">
         <v>1036.77</v>
@@ -1493,16 +1489,16 @@
         <v>2351.1174999999998</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1523,16 +1519,16 @@
         <v>2300</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1553,24 +1549,24 @@
         <v>2875</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="1">
         <v>1115.56</v>
@@ -1583,24 +1579,24 @@
         <v>2530</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="1">
         <v>1046.06</v>
@@ -1613,24 +1609,24 @@
         <v>2875</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1">
         <v>1154.93</v>
@@ -1643,16 +1639,16 @@
         <v>2633.6609999999996</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1673,13 +1669,13 @@
         <v>1856.2839999999999</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1701,22 +1697,22 @@
         <v>2134.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C17" s="1">
         <v>1170.92</v>
@@ -1729,20 +1725,20 @@
         <v>2231</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C18" s="1">
         <v>963.69500000000005</v>
@@ -1755,20 +1751,20 @@
         <v>3300.0054999999998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C19" s="1">
         <v>1163.49</v>
@@ -1781,48 +1777,48 @@
         <v>3399.9979999999996</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="A20" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="8">
         <v>290</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="8">
         <v>380</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="8">
         <f t="shared" si="2"/>
         <v>436.99999999999994</v>
       </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>196</v>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C21" s="1">
         <v>201.5</v>
@@ -1838,17 +1834,17 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C22" s="1">
         <v>69.69</v>
@@ -1864,17 +1860,17 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C23" s="1">
         <v>21.476064999999998</v>
@@ -1890,17 +1886,17 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C24" s="1">
         <v>61.337499999999999</v>
@@ -1916,7 +1912,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
@@ -1926,7 +1922,7 @@
         <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C25" s="1">
         <v>36.6</v>
@@ -1942,10 +1938,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -1954,7 +1950,7 @@
         <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C26" s="1">
         <v>109</v>
@@ -1970,19 +1966,19 @@
         <v>3</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C27" s="1">
         <v>24.002386000000001</v>
@@ -1995,7 +1991,7 @@
         <v>78.602499999999992</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G27" s="1" t="b">
         <v>1</v>
@@ -2023,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2049,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2075,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2101,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="1"/>
@@ -2315,156 +2311,156 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="8">
         <v>2.5</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="12">
         <v>2.61</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="8">
         <f t="shared" ref="E40:E47" si="6">+D40*1.15</f>
         <v>3.0014999999999996</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="8">
         <v>20</v>
       </c>
-      <c r="G40" s="1" t="b">
+      <c r="G40" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="8">
         <v>15.8</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="12">
         <v>14.51</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="8">
         <f t="shared" si="6"/>
         <v>16.686499999999999</v>
       </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1" t="b">
+      <c r="F41" s="8">
+        <v>1</v>
+      </c>
+      <c r="G41" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="8">
         <v>135.4</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="12">
         <v>176.52</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="8">
         <f t="shared" si="6"/>
         <v>202.99799999999999</v>
       </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1" t="b">
+      <c r="F42" s="8">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="8">
         <v>50</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="12">
         <v>65.22</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="8">
         <f t="shared" si="6"/>
         <v>75.002999999999986</v>
       </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1" t="b">
+      <c r="F43" s="8">
+        <v>1</v>
+      </c>
+      <c r="G43" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="8">
         <v>26.9</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="12">
         <v>33.909999999999997</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="8">
         <f t="shared" si="6"/>
         <v>38.99649999999999</v>
       </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1" t="b">
+      <c r="F44" s="8">
+        <v>1</v>
+      </c>
+      <c r="G44" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="8">
         <v>6.1</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="12">
         <v>5.61</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="8">
         <f t="shared" si="6"/>
         <v>6.4515000000000002</v>
       </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1" t="b">
+      <c r="F45" s="8">
+        <v>1</v>
+      </c>
+      <c r="G45" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H45" s="1"/>
@@ -2488,7 +2484,7 @@
         <v>1.5984999999999998</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>1</v>
@@ -2627,55 +2623,55 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="C52" s="8">
+      <c r="A52" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" s="14">
         <v>0.44</v>
       </c>
-      <c r="D52" s="12">
+      <c r="D52" s="15">
         <v>1.6</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="14">
         <f t="shared" si="7"/>
         <v>1.8399999999999999</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="H52" s="8"/>
+      <c r="F52" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" s="14"/>
       <c r="I52" s="8"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="14">
         <v>2.27</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D53" s="15">
         <v>4.1900000000000004</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="14">
         <f t="shared" si="7"/>
         <v>4.8185000000000002</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="H53" s="8"/>
+      <c r="F53" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="H53" s="14"/>
       <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9">
@@ -2903,7 +2899,7 @@
         <v>2.5644999999999998</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G62" s="1" t="b">
         <v>1</v>
@@ -2929,7 +2925,7 @@
         <v>18.894499999999997</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G63" s="1" t="b">
         <v>1</v>
@@ -2955,7 +2951,7 @@
         <v>8.4640000000000004</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G64" s="1" t="b">
         <v>1</v>
@@ -2981,7 +2977,7 @@
         <v>8.4640000000000004</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G65" s="1" t="b">
         <v>1</v>
@@ -3003,17 +2999,17 @@
         <v>1794</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" ref="E66:E82" si="9">+D66*1.15</f>
+        <f t="shared" ref="E66:E81" si="9">+D66*1.15</f>
         <v>2063.1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I66" s="1"/>
     </row>
@@ -3191,7 +3187,7 @@
         <v>9.7979999999999983</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G73" s="1" t="b">
         <v>1</v>
@@ -3200,517 +3196,517 @@
       <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C74" s="8">
+      <c r="C74" s="14">
         <v>7.25</v>
       </c>
-      <c r="D74" s="12">
+      <c r="D74" s="15">
         <v>31.25</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E74" s="14">
         <f t="shared" si="9"/>
         <v>35.9375</v>
       </c>
-      <c r="F74" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="G74" s="8" t="b">
+      <c r="F74" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G74" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="14">
         <v>31.195667</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D75" s="15">
         <v>84.82</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="14">
         <f t="shared" si="9"/>
         <v>97.542999999999978</v>
       </c>
-      <c r="F75" s="1">
-        <v>1</v>
-      </c>
-      <c r="G75" s="1" t="b">
+      <c r="F75" s="14">
+        <v>1</v>
+      </c>
+      <c r="G75" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="14">
         <v>100.704865</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D76" s="15">
         <v>321.74</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="14">
         <f t="shared" si="9"/>
         <v>370.00099999999998</v>
       </c>
-      <c r="F76" s="1">
-        <v>1</v>
-      </c>
-      <c r="G76" s="1" t="b">
+      <c r="F76" s="14">
+        <v>1</v>
+      </c>
+      <c r="G76" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="14">
         <v>82.356999999999999</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D77" s="15">
         <v>357.14</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="14">
         <f t="shared" si="9"/>
         <v>410.71099999999996</v>
       </c>
-      <c r="F77" s="1">
-        <v>1</v>
-      </c>
-      <c r="G77" s="1" t="b">
+      <c r="F77" s="14">
+        <v>1</v>
+      </c>
+      <c r="G77" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C78" s="14">
         <v>3.872404</v>
       </c>
-      <c r="D78" s="12">
+      <c r="D78" s="15">
         <v>16.07</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E78" s="14">
         <f t="shared" si="9"/>
         <v>18.480499999999999</v>
       </c>
-      <c r="F78" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G78" s="8" t="b">
+      <c r="F78" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G78" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="C79" s="8">
+      <c r="C79" s="14">
         <v>16.879968999999999</v>
       </c>
-      <c r="D79" s="12">
+      <c r="D79" s="15">
         <v>19.57</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E79" s="14">
         <f t="shared" si="9"/>
         <v>22.505499999999998</v>
       </c>
-      <c r="F79" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G79" s="8" t="b">
+      <c r="F79" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G79" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C80" s="1">
-        <v>6.7</v>
-      </c>
-      <c r="D80" s="4">
-        <v>16.07</v>
-      </c>
-      <c r="E80" s="1">
+      <c r="C80" s="14">
+        <v>36.583019</v>
+      </c>
+      <c r="D80" s="15">
+        <v>104.35</v>
+      </c>
+      <c r="E80" s="14">
         <f t="shared" si="9"/>
-        <v>18.480499999999999</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G80" s="1" t="b">
+        <v>120.00249999999998</v>
+      </c>
+      <c r="F80" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G80" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="1">
-        <v>36.583019</v>
-      </c>
-      <c r="D81" s="4">
-        <v>104.35</v>
-      </c>
-      <c r="E81" s="1">
+      <c r="C81" s="14">
+        <v>56.479194999999997</v>
+      </c>
+      <c r="D81" s="15">
+        <v>140.18</v>
+      </c>
+      <c r="E81" s="14">
         <f t="shared" si="9"/>
-        <v>120.00249999999998</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="G81" s="1" t="b">
+        <v>161.20699999999999</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="G81" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C82" s="8">
-        <v>56.479194999999997</v>
-      </c>
-      <c r="D82" s="12">
-        <v>140.18</v>
-      </c>
-      <c r="E82" s="8">
-        <f t="shared" si="9"/>
-        <v>161.20699999999999</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="G82" s="8" t="b">
+      <c r="C82" s="14">
+        <v>300</v>
+      </c>
+      <c r="D82" s="15">
+        <v>300</v>
+      </c>
+      <c r="E82" s="14">
+        <v>300</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G82" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C83" s="1">
-        <v>300</v>
-      </c>
-      <c r="D83" s="4">
-        <v>300</v>
-      </c>
-      <c r="E83" s="1">
-        <v>300</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G83" s="1" t="b">
+      <c r="C83" s="14">
+        <v>240.5</v>
+      </c>
+      <c r="D83" s="15">
+        <v>358.8</v>
+      </c>
+      <c r="E83" s="14">
+        <f t="shared" ref="E83:E95" si="10">+D83*1.15</f>
+        <v>412.62</v>
+      </c>
+      <c r="F83" s="14">
+        <v>1</v>
+      </c>
+      <c r="G83" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C84" s="1">
-        <v>240.5</v>
-      </c>
-      <c r="D84" s="4">
-        <v>358.8</v>
-      </c>
-      <c r="E84" s="1">
-        <f t="shared" ref="E84:E96" si="10">+D84*1.15</f>
-        <v>412.62</v>
-      </c>
-      <c r="F84" s="1">
-        <v>1</v>
-      </c>
-      <c r="G84" s="1" t="b">
+      <c r="C84" s="14">
+        <v>0</v>
+      </c>
+      <c r="D84" s="15">
+        <v>112.32</v>
+      </c>
+      <c r="E84" s="14">
+        <f t="shared" si="10"/>
+        <v>129.16799999999998</v>
+      </c>
+      <c r="F84" s="14">
+        <v>1</v>
+      </c>
+      <c r="G84" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C85" s="1">
-        <v>0</v>
-      </c>
-      <c r="D85" s="4">
-        <v>112.32</v>
-      </c>
-      <c r="E85" s="1">
+      <c r="C85" s="14">
+        <v>4</v>
+      </c>
+      <c r="D85" s="15">
+        <v>16</v>
+      </c>
+      <c r="E85" s="14">
         <f t="shared" si="10"/>
-        <v>129.16799999999998</v>
-      </c>
-      <c r="F85" s="1">
-        <v>1</v>
-      </c>
-      <c r="G85" s="1" t="b">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="F85" s="14">
+        <v>2</v>
+      </c>
+      <c r="G85" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="D86" s="15">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="E86" s="14">
+        <f t="shared" si="10"/>
+        <v>19.043999999999997</v>
+      </c>
+      <c r="F86" s="14">
         <v>4</v>
       </c>
-      <c r="D86" s="4">
-        <v>16</v>
-      </c>
-      <c r="E86" s="1">
-        <f t="shared" si="10"/>
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F86" s="1">
-        <v>2</v>
-      </c>
-      <c r="G86" s="1" t="b">
+      <c r="G86" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C87" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="D87" s="4">
-        <v>16.559999999999999</v>
-      </c>
-      <c r="E87" s="1">
+      <c r="C87" s="14">
+        <v>5.89</v>
+      </c>
+      <c r="D87" s="15">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="E87" s="14">
         <f t="shared" si="10"/>
-        <v>19.043999999999997</v>
-      </c>
-      <c r="F87" s="1">
-        <v>4</v>
-      </c>
-      <c r="G87" s="1" t="b">
+        <v>9.5219999999999985</v>
+      </c>
+      <c r="F87" s="14">
+        <v>2</v>
+      </c>
+      <c r="G87" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C88" s="1">
-        <v>5.89</v>
-      </c>
-      <c r="D88" s="4">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="E88" s="1">
+      <c r="C88" s="14">
+        <v>60</v>
+      </c>
+      <c r="D88" s="15">
+        <v>134.78</v>
+      </c>
+      <c r="E88" s="14">
         <f t="shared" si="10"/>
-        <v>9.5219999999999985</v>
-      </c>
-      <c r="F88" s="1">
-        <v>2</v>
-      </c>
-      <c r="G88" s="1" t="b">
+        <v>154.99699999999999</v>
+      </c>
+      <c r="F88" s="14">
+        <v>1</v>
+      </c>
+      <c r="G88" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C89" s="1">
-        <v>60</v>
-      </c>
-      <c r="D89" s="4">
-        <v>134.78</v>
-      </c>
-      <c r="E89" s="1">
+      <c r="A89" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" s="14">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="D89" s="15">
+        <v>21.74</v>
+      </c>
+      <c r="E89" s="14">
         <f t="shared" si="10"/>
-        <v>154.99699999999999</v>
-      </c>
-      <c r="F89" s="1">
-        <v>1</v>
-      </c>
-      <c r="G89" s="1" t="b">
+        <v>25.000999999999998</v>
+      </c>
+      <c r="F89" s="14">
+        <v>4</v>
+      </c>
+      <c r="G89" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C90" s="1">
-        <v>8.7100000000000009</v>
-      </c>
-      <c r="D90" s="4">
-        <v>21.74</v>
-      </c>
-      <c r="E90" s="1">
+      <c r="C90" s="14">
+        <v>3.55</v>
+      </c>
+      <c r="D90" s="15">
+        <v>8.48</v>
+      </c>
+      <c r="E90" s="14">
         <f t="shared" si="10"/>
-        <v>25.000999999999998</v>
-      </c>
-      <c r="F90" s="1">
-        <v>4</v>
-      </c>
-      <c r="G90" s="1" t="b">
+        <v>9.7519999999999989</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G90" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C91" s="8">
-        <v>3.55</v>
-      </c>
-      <c r="D91" s="12">
-        <v>8.48</v>
-      </c>
-      <c r="E91" s="8">
+      <c r="C91" s="14">
+        <v>61.337499999999999</v>
+      </c>
+      <c r="D91" s="15">
+        <v>252.17</v>
+      </c>
+      <c r="E91" s="14">
         <f t="shared" si="10"/>
-        <v>9.7519999999999989</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="G91" s="1" t="b">
+        <v>289.99549999999994</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G91" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C92" s="8">
-        <v>61.337499999999999</v>
-      </c>
-      <c r="D92" s="12">
-        <v>252.17</v>
-      </c>
-      <c r="E92" s="8">
+      <c r="C92" s="14">
+        <v>80</v>
+      </c>
+      <c r="D92" s="15">
+        <v>80</v>
+      </c>
+      <c r="E92" s="14">
         <f t="shared" si="10"/>
-        <v>289.99549999999994</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="G92" s="1" t="b">
+        <v>92</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="G92" s="14" t="b">
         <v>1</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C93" s="8">
-        <v>80</v>
-      </c>
-      <c r="D93" s="12">
-        <v>80</v>
-      </c>
-      <c r="E93" s="8">
+      <c r="A93" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C93" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D93" s="4">
+        <v>6</v>
+      </c>
+      <c r="E93" s="1">
         <f t="shared" si="10"/>
-        <v>92</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>241</v>
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1</v>
       </c>
       <c r="G93" s="1" t="b">
         <v>1</v>
@@ -3720,13 +3716,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C94" s="1">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D94" s="4">
         <v>6</v>
@@ -3745,60 +3741,34 @@
       <c r="I94" s="1"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C95" s="1">
-        <v>6</v>
-      </c>
-      <c r="D95" s="4">
-        <v>6</v>
-      </c>
-      <c r="E95" s="1">
+      <c r="A95" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C95" s="8">
+        <v>800</v>
+      </c>
+      <c r="D95" s="12">
+        <v>1500</v>
+      </c>
+      <c r="E95" s="8">
         <f t="shared" si="10"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="F95" s="1">
-        <v>1</v>
-      </c>
-      <c r="G95" s="1" t="b">
+        <v>1724.9999999999998</v>
+      </c>
+      <c r="F95" s="8">
+        <v>1</v>
+      </c>
+      <c r="G95" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="C96" s="8">
-        <v>800</v>
-      </c>
-      <c r="D96" s="12">
-        <v>1500</v>
-      </c>
-      <c r="E96" s="8">
-        <f t="shared" si="10"/>
-        <v>1724.9999999999998</v>
-      </c>
-      <c r="F96" s="8">
-        <v>1</v>
-      </c>
-      <c r="G96" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-    </row>
-    <row r="100" spans="2:2">
-      <c r="B100" t="s">
-        <v>225</v>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates on invoice.app, etl adn exel
</commit_message>
<xml_diff>
--- a/Elevators.xlsx
+++ b/Elevators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Desktop/Invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5E621A-73A6-A745-BEAE-8963C91A13F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AF4DF7-728D-A047-85DA-EEEDDB29825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="212">
   <si>
     <t>part_id</t>
   </si>
@@ -146,12 +146,6 @@
     <t>ASC 056</t>
   </si>
   <si>
-    <t>ASC008</t>
-  </si>
-  <si>
-    <t>AMORTIGUADOR 540 ESPECIAL PUARSA</t>
-  </si>
-  <si>
     <t>ASC052</t>
   </si>
   <si>
@@ -221,12 +215,6 @@
     <t>FINAL DE CARRERA  CONTACTO CERRADO</t>
   </si>
   <si>
-    <t>ASC516</t>
-  </si>
-  <si>
-    <t>RELES 24 VOLTIOS PARA PUERTAS</t>
-  </si>
-  <si>
     <t>ASC522</t>
   </si>
   <si>
@@ -293,12 +281,6 @@
     <t>CAMISA DE TRABAJO JEAN</t>
   </si>
   <si>
-    <t>CERRADURA</t>
-  </si>
-  <si>
-    <t>CERRADURA PUERTA BATIENTE</t>
-  </si>
-  <si>
     <t>CONTROL HEYTECH 7.5kw sin encoder</t>
   </si>
   <si>
@@ -443,12 +425,6 @@
     <t>CUÑA RETRACTIL</t>
   </si>
   <si>
-    <t>ON-03 LIFT DOOR</t>
-  </si>
-  <si>
-    <t>CHAPA PARA PUERTA MANUAL</t>
-  </si>
-  <si>
     <t>ONKP-01CAR</t>
   </si>
   <si>
@@ -461,12 +437,6 @@
     <t>ACEITERO PEQUEÑO</t>
   </si>
   <si>
-    <t>PAK210</t>
-  </si>
-  <si>
-    <t>POLEA DE METAL 210*5*8</t>
-  </si>
-  <si>
     <t>PESASKMON</t>
   </si>
   <si>
@@ -599,9 +569,6 @@
     <t>450kg</t>
   </si>
   <si>
-    <t>hydraulic_cylinder</t>
-  </si>
-  <si>
     <t>not machine_room and not hydraulic_cylinder</t>
   </si>
   <si>
@@ -650,21 +617,12 @@
     <t>CABLE DE ACERO # 8 MM</t>
   </si>
   <si>
-    <t>3*F</t>
-  </si>
-  <si>
-    <t>2 if machine_room and not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 3</t>
-  </si>
-  <si>
     <t>ceil(0.6 * F) if (not machine_room and not hydraulic_cylinder and ((12 &lt; P &lt; 14) or (13 &lt; P &lt;= 16))) else 0</t>
   </si>
   <si>
     <t>ceil(1.4 * F) if (not hydraulic_cylinder and (P &lt;= 3 or (6 &lt; P &lt; 10))) else 0</t>
   </si>
   <si>
-    <t>2 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 4</t>
-  </si>
-  <si>
     <t>0 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else F</t>
   </si>
   <si>
@@ -674,10 +632,46 @@
     <t>0 if not hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 1</t>
   </si>
   <si>
-    <t>(not machine_room) and ((P &lt;= 3) or (6 &lt; P &lt; 10))</t>
-  </si>
-  <si>
-    <t>machine_room and ((P &lt;= 3) or (6 &lt; P &lt; 10))</t>
+    <t>TARJETA DE PROXIMIDAD ESTANDAR 256L</t>
+  </si>
+  <si>
+    <t>TARJ20</t>
+  </si>
+  <si>
+    <t>1.4*F</t>
+  </si>
+  <si>
+    <t>ceil(5*F)</t>
+  </si>
+  <si>
+    <t>2 if hydraulic_cylinder and ((P &lt;= 3) or (6 &lt; P &lt; 10)) else 4</t>
+  </si>
+  <si>
+    <t>0 if hydraulic_cylinder else 20</t>
+  </si>
+  <si>
+    <t>1 if hydraulic_cylinder else 0</t>
+  </si>
+  <si>
+    <t>0 if hydraulic_cylinder else 1</t>
+  </si>
+  <si>
+    <t>2 if hydraulic_cylinder else 0</t>
+  </si>
+  <si>
+    <t>0 if hydraulic_cylinder else ceil(6*F)</t>
+  </si>
+  <si>
+    <t>2 if hydraulic_cylinder else 3</t>
+  </si>
+  <si>
+    <t>GYE02</t>
+  </si>
+  <si>
+    <t>INSTALACION MECANICA ASCENSOR HIDRAULICO</t>
+  </si>
+  <si>
+    <t>0 if hydraulic_cylinder else F</t>
   </si>
 </sst>
 </file>
@@ -769,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -783,6 +777,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B74E1E-2FAB-A84A-BD4C-ED601BD34DA2}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="125" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="98" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1182,16 +1178,16 @@
         <v>3475.5529999999994</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1212,16 +1208,16 @@
         <v>3679.9999999999995</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1242,16 +1238,16 @@
         <v>2964.4470000000001</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1272,16 +1268,16 @@
         <v>3577.7764999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1302,16 +1298,16 @@
         <v>3085.1279999999997</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1332,16 +1328,16 @@
         <v>3986.6704999999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1349,7 +1345,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C8" s="1">
         <v>2534.1733330000002</v>
@@ -1362,16 +1358,16 @@
         <v>4499.9959999999992</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1379,7 +1375,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C9" s="1">
         <v>1036.77</v>
@@ -1392,16 +1388,16 @@
         <v>2351.1174999999998</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1422,16 +1418,16 @@
         <v>2300</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1452,24 +1448,24 @@
         <v>2875</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C12" s="1">
         <v>1115.56</v>
@@ -1482,24 +1478,24 @@
         <v>2530</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C13" s="1">
         <v>1046.06</v>
@@ -1512,24 +1508,24 @@
         <v>2875</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1">
         <v>1154.93</v>
@@ -1542,24 +1538,24 @@
         <v>2633.6609999999996</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1">
         <v>1170.92</v>
@@ -1572,22 +1568,22 @@
         <v>1856.2839999999999</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1">
         <v>1444.15</v>
@@ -1600,22 +1596,22 @@
         <v>2134.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C17" s="1">
         <v>1170.92</v>
@@ -1624,24 +1620,24 @@
         <v>1940</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ref="E17:E23" si="2">+D17*1.15</f>
+        <f t="shared" ref="E17:E22" si="2">+D17*1.15</f>
         <v>2231</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C18" s="1">
         <v>963.69500000000005</v>
@@ -1654,20 +1650,20 @@
         <v>3300.0054999999998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C19" s="1">
         <v>1163.49</v>
@@ -1680,20 +1676,20 @@
         <v>3399.9979999999996</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C20" s="6">
         <v>290</v>
@@ -1712,16 +1708,16 @@
         <v>1</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C21" s="1">
         <v>201.5</v>
@@ -1737,17 +1733,17 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1">
         <v>69.69</v>
@@ -1763,249 +1759,262 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C23" s="1">
-        <v>21.476064999999998</v>
+        <v>36.6</v>
       </c>
       <c r="D23" s="1">
-        <v>49.57</v>
+        <v>67.34</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="2"/>
-        <v>57.005499999999998</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>2</v>
+        <f>+D23*1.15</f>
+        <v>77.441000000000003</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="1">
+        <v>109</v>
+      </c>
+      <c r="D24" s="1">
+        <v>200.56</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" ref="E24" si="3">+D24*1.15</f>
+        <v>230.64399999999998</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1">
-        <v>36.6</v>
-      </c>
-      <c r="D25" s="1">
-        <v>67.34</v>
+        <v>24.002386000000001</v>
+      </c>
+      <c r="D25" s="3">
+        <v>68.349999999999994</v>
       </c>
       <c r="E25" s="1">
         <f>+D25*1.15</f>
-        <v>77.441000000000003</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>155</v>
+        <v>78.602499999999992</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G25" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1">
-        <v>109</v>
-      </c>
-      <c r="D26" s="1">
-        <v>200.56</v>
+        <v>182.813333</v>
+      </c>
+      <c r="D26" s="3">
+        <v>375</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26" si="3">+D26*1.15</f>
-        <v>230.64399999999998</v>
-      </c>
-      <c r="F26" s="1">
-        <v>3</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>155</v>
-      </c>
+        <f>+D26*1.15</f>
+        <v>431.24999999999994</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
-        <v>24.002386000000001</v>
+        <v>533.625</v>
       </c>
       <c r="D27" s="3">
-        <v>68.349999999999994</v>
+        <v>1304.3499999999999</v>
       </c>
       <c r="E27" s="1">
         <f>+D27*1.15</f>
-        <v>78.602499999999992</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>1500.0024999999998</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1">
-        <v>182.813333</v>
+        <v>99.29</v>
       </c>
       <c r="D28" s="3">
-        <v>375</v>
+        <v>275</v>
       </c>
       <c r="E28" s="1">
         <f>+D28*1.15</f>
-        <v>431.24999999999994</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>2</v>
+        <v>316.25</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1">
-        <v>533.625</v>
+        <v>126.91249999999999</v>
       </c>
       <c r="D29" s="3">
-        <v>1304.3499999999999</v>
+        <v>326.93</v>
       </c>
       <c r="E29" s="1">
         <f>+D29*1.15</f>
-        <v>1500.0024999999998</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
+        <v>375.96949999999998</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>99.29</v>
+        <v>50.158729999999998</v>
       </c>
       <c r="D30" s="3">
-        <v>275</v>
+        <v>114</v>
       </c>
       <c r="E30" s="1">
-        <f>+D30*1.15</f>
-        <v>316.25</v>
+        <f t="shared" ref="E30:E31" si="4">+D30*1.15</f>
+        <v>131.1</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>192</v>
+      <c r="G30" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1">
-        <v>126.91249999999999</v>
-      </c>
-      <c r="D31" s="3">
-        <v>326.93</v>
+        <v>4.2275</v>
+      </c>
+      <c r="D31" s="4">
+        <v>9.1999999999999993</v>
       </c>
       <c r="E31" s="1">
-        <f>+D31*1.15</f>
-        <v>375.96949999999998</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>192</v>
+        <f t="shared" si="4"/>
+        <v>10.579999999999998</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1">
-        <v>50.158729999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D32" s="3">
-        <v>114</v>
+        <v>4.07</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" ref="E32:E33" si="4">+D32*1.15</f>
-        <v>131.1</v>
+        <f>+D32*1.15</f>
+        <v>4.6805000000000003</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -2013,51 +2022,51 @@
       <c r="G32" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1">
-        <v>4.2275</v>
-      </c>
-      <c r="D33" s="4">
-        <v>9.1999999999999993</v>
+        <v>0.3</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.8</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="4"/>
-        <v>10.579999999999998</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1</v>
+        <f t="shared" ref="E33:E34" si="5">+D33*1.15</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="G33" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1">
-        <v>2.2000000000000002</v>
+        <v>19</v>
       </c>
       <c r="D34" s="3">
-        <v>4.07</v>
+        <v>34.96</v>
       </c>
       <c r="E34" s="1">
-        <f>+D34*1.15</f>
-        <v>4.6805000000000003</v>
+        <f t="shared" si="5"/>
+        <v>40.204000000000001</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -2066,157 +2075,157 @@
         <v>1</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>13.708636</v>
       </c>
       <c r="D35" s="3">
-        <v>1.39</v>
+        <v>32.86</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" ref="E35:E36" si="5">+D35*1.15</f>
-        <v>1.5984999999999998</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>170</v>
+        <f t="shared" ref="E35:E44" si="6">+D35*1.15</f>
+        <v>37.788999999999994</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
       </c>
       <c r="G35" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="5"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1">
-        <v>19</v>
+        <v>500</v>
       </c>
       <c r="D36" s="3">
-        <v>34.96</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="5"/>
-        <v>40.204000000000001</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+        <v>460</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="6"/>
+        <v>529</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1">
-        <v>19.096</v>
+        <v>2.99</v>
       </c>
       <c r="D37" s="3">
-        <v>5.82</v>
+        <v>13.4</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" ref="E37:E47" si="6">+D37*1.15</f>
-        <v>6.6929999999999996</v>
-      </c>
-      <c r="F37" s="1" t="s">
+        <f t="shared" si="6"/>
+        <v>15.409999999999998</v>
+      </c>
+      <c r="F37" s="1">
         <v>2</v>
       </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="5"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>192</v>
       </c>
       <c r="C38" s="1">
-        <v>13.708636</v>
+        <v>0.44</v>
       </c>
       <c r="D38" s="3">
-        <v>32.86</v>
+        <v>1.6</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="6"/>
-        <v>37.788999999999994</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2</v>
-      </c>
-      <c r="G38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="2"/>
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C39" s="1">
-        <v>500</v>
+        <v>2.27</v>
       </c>
       <c r="D39" s="3">
-        <v>460</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="6"/>
-        <v>529</v>
-      </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1" t="b">
-        <v>1</v>
+        <v>4.8185000000000002</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C40" s="1">
-        <v>2.99</v>
+        <v>157.99333300000001</v>
       </c>
       <c r="D40" s="3">
-        <v>13.4</v>
+        <v>401.79</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="6"/>
-        <v>15.409999999999998</v>
+        <v>462.05849999999998</v>
       </c>
       <c r="F40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
@@ -2226,75 +2235,75 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>202</v>
+        <v>51</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>203</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1">
-        <v>0.44</v>
+        <v>13.108750000000001</v>
       </c>
       <c r="D41" s="3">
-        <v>1.6</v>
+        <v>53.57</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="6"/>
-        <v>1.8399999999999999</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>164</v>
+        <v>61.605499999999992</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1">
-        <v>2.27</v>
+        <v>56.094999999999999</v>
       </c>
       <c r="D42" s="3">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="E42" s="1">
+        <v>98.57</v>
+      </c>
+      <c r="E42" s="6">
         <f t="shared" si="6"/>
-        <v>4.8185000000000002</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>155</v>
+        <v>113.35549999999998</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G42" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1">
-        <v>157.99333300000001</v>
+        <v>45.5</v>
       </c>
       <c r="D43" s="3">
-        <v>401.79</v>
+        <v>100</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="6"/>
-        <v>462.05849999999998</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="G43" s="1" t="b">
         <v>1</v>
@@ -2304,23 +2313,23 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C44" s="1">
-        <v>13.108750000000001</v>
+        <v>2.3317999999999999</v>
       </c>
       <c r="D44" s="3">
-        <v>53.57</v>
+        <v>7.83</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="6"/>
-        <v>61.605499999999992</v>
+        <v>9.0045000000000002</v>
       </c>
       <c r="F44" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G44" s="1" t="b">
         <v>1</v>
@@ -2330,23 +2339,23 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C45" s="1">
-        <v>56.094999999999999</v>
+        <v>427</v>
       </c>
       <c r="D45" s="3">
-        <v>98.57</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="6"/>
-        <v>113.35549999999998</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
+        <v>736</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" ref="E45:E50" si="7">+D45*1.15</f>
+        <v>846.4</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="G45" s="1" t="b">
         <v>1</v>
@@ -2356,23 +2365,23 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1">
-        <v>45.5</v>
+        <v>14.5</v>
       </c>
       <c r="D46" s="3">
-        <v>100</v>
+        <v>40.869999999999997</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="6"/>
-        <v>114.99999999999999</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>47.000499999999995</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>1</v>
@@ -2382,23 +2391,23 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1">
-        <v>2.3317999999999999</v>
+        <v>1.6983000000000002E-2</v>
       </c>
       <c r="D47" s="3">
-        <v>7.83</v>
+        <v>2.23</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="6"/>
-        <v>9.0045000000000002</v>
-      </c>
-      <c r="F47" s="1">
-        <v>6</v>
+        <f t="shared" si="7"/>
+        <v>2.5644999999999998</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="G47" s="1" t="b">
         <v>1</v>
@@ -2407,23 +2416,24 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="5">
-        <v>11.78</v>
-      </c>
-      <c r="D48" s="4">
-        <v>10.84</v>
-      </c>
-      <c r="E48" s="5">
-        <v>12.463240000000001</v>
-      </c>
-      <c r="F48" s="5">
-        <v>4</v>
+      <c r="A48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1.159999</v>
+      </c>
+      <c r="D48" s="3">
+        <v>16.43</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="7"/>
+        <v>18.894499999999997</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="G48" s="1" t="b">
         <v>1</v>
@@ -2433,23 +2443,23 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1">
-        <v>427</v>
+        <v>5</v>
       </c>
       <c r="D49" s="3">
-        <v>736</v>
+        <v>7.36</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" ref="E49:E54" si="7">+D49*1.15</f>
-        <v>846.4</v>
-      </c>
-      <c r="F49" s="1">
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="G49" s="1" t="b">
         <v>1</v>
@@ -2459,23 +2469,23 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C50" s="1">
-        <v>14.5</v>
+        <v>5</v>
       </c>
       <c r="D50" s="3">
-        <v>40.869999999999997</v>
+        <v>7.36</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="7"/>
-        <v>47.000499999999995</v>
-      </c>
-      <c r="F50" s="1">
-        <v>1</v>
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="G50" s="1" t="b">
         <v>1</v>
@@ -2485,101 +2495,101 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C51" s="1">
-        <v>1.6983000000000002E-2</v>
+        <v>975</v>
       </c>
       <c r="D51" s="3">
-        <v>2.23</v>
+        <v>1794</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="7"/>
-        <v>2.5644999999999998</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G51" s="1" t="b">
-        <v>1</v>
+        <f t="shared" ref="E51:E64" si="8">+D51*1.15</f>
+        <v>2063.1</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C52" s="1">
-        <v>1.159999</v>
+        <v>15.65</v>
       </c>
       <c r="D52" s="3">
-        <v>16.43</v>
+        <v>35.71</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="7"/>
-        <v>18.894499999999997</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>169</v>
+        <f t="shared" si="8"/>
+        <v>41.066499999999998</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="G52" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H52" s="1"/>
+      <c r="H52" s="11"/>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C53" s="1">
-        <v>5</v>
+        <v>11.55</v>
       </c>
       <c r="D53" s="3">
-        <v>7.36</v>
+        <v>12.24</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="7"/>
-        <v>8.4640000000000004</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>167</v>
+        <f t="shared" si="8"/>
+        <v>14.075999999999999</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2</v>
       </c>
       <c r="G53" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H53" s="1"/>
-      <c r="I53" s="6"/>
+      <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D54" s="3">
-        <v>7.36</v>
+        <v>120</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="7"/>
-        <v>8.4640000000000004</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>167</v>
+        <f t="shared" si="8"/>
+        <v>138</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
       </c>
       <c r="G54" s="1" t="b">
         <v>1</v>
@@ -2589,51 +2599,49 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1">
-        <v>975</v>
+        <v>3.6944720000000002</v>
       </c>
       <c r="D55" s="3">
-        <v>1794</v>
+        <v>8.52</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" ref="E55:E68" si="8">+D55*1.15</f>
-        <v>2063.1</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>187</v>
-      </c>
+        <f t="shared" si="8"/>
+        <v>9.7979999999999983</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C56" s="1">
-        <v>15.65</v>
+        <v>7.25</v>
       </c>
       <c r="D56" s="3">
-        <v>35.71</v>
+        <v>31.25</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="8"/>
-        <v>41.066499999999998</v>
-      </c>
-      <c r="F56" s="1">
-        <v>1</v>
+        <v>35.9375</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="G56" s="1" t="b">
         <v>1</v>
@@ -2643,23 +2651,23 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C57" s="1">
-        <v>11.55</v>
+        <v>31.195667</v>
       </c>
       <c r="D57" s="3">
-        <v>12.24</v>
-      </c>
-      <c r="E57" s="1">
+        <v>84.82</v>
+      </c>
+      <c r="E57" s="6">
         <f t="shared" si="8"/>
-        <v>14.075999999999999</v>
-      </c>
-      <c r="F57" s="1">
-        <v>2</v>
+        <v>97.542999999999978</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="G57" s="1" t="b">
         <v>1</v>
@@ -2669,23 +2677,23 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C58" s="1">
-        <v>18.78</v>
+        <v>100.704865</v>
       </c>
       <c r="D58" s="3">
-        <v>45.18</v>
-      </c>
-      <c r="E58" s="1">
+        <v>321.74</v>
+      </c>
+      <c r="E58" s="6">
         <f t="shared" si="8"/>
-        <v>51.956999999999994</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>2</v>
+        <v>370.00099999999998</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="G58" s="1" t="b">
         <v>1</v>
@@ -2695,23 +2703,23 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1">
-        <v>138</v>
+        <v>82.356999999999999</v>
       </c>
       <c r="D59" s="3">
-        <v>164.31</v>
-      </c>
-      <c r="E59" s="1">
+        <v>357.14</v>
+      </c>
+      <c r="E59" s="6">
         <f t="shared" si="8"/>
-        <v>188.95649999999998</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1</v>
+        <v>410.71099999999996</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="G59" s="1" t="b">
         <v>1</v>
@@ -2721,75 +2729,75 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C60" s="1">
-        <v>3.6944720000000002</v>
+        <v>3.872404</v>
       </c>
       <c r="D60" s="3">
-        <v>8.52</v>
-      </c>
-      <c r="E60" s="1">
+        <v>16.07</v>
+      </c>
+      <c r="E60" s="6">
         <f t="shared" si="8"/>
-        <v>9.7979999999999983</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G60" s="1" t="b">
-        <v>1</v>
+        <v>18.480499999999999</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C61" s="1">
-        <v>7.25</v>
+        <v>16.879968999999999</v>
       </c>
       <c r="D61" s="3">
-        <v>31.25</v>
+        <v>19.57</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="8"/>
-        <v>35.9375</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G61" s="1" t="b">
-        <v>1</v>
+        <v>22.505499999999998</v>
+      </c>
+      <c r="F61" s="1">
+        <v>10</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C62" s="1">
-        <v>31.195667</v>
+        <v>36.583019</v>
       </c>
       <c r="D62" s="3">
-        <v>84.82</v>
+        <v>104.35</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" si="8"/>
-        <v>97.542999999999978</v>
-      </c>
-      <c r="F62" s="1">
-        <v>1</v>
+        <v>120.00249999999998</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="G62" s="1" t="b">
         <v>1</v>
@@ -2799,23 +2807,23 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C63" s="1">
-        <v>100.704865</v>
+        <v>56.479194999999997</v>
       </c>
       <c r="D63" s="3">
-        <v>321.74</v>
+        <v>140.18</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" si="8"/>
-        <v>370.00099999999998</v>
-      </c>
-      <c r="F63" s="1">
-        <v>1</v>
+        <v>161.20699999999999</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="G63" s="1" t="b">
         <v>1</v>
@@ -2825,101 +2833,97 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>102</v>
+        <v>210</v>
       </c>
       <c r="C64" s="1">
-        <v>82.356999999999999</v>
+        <v>350</v>
       </c>
       <c r="D64" s="3">
-        <v>357.14</v>
+        <v>350</v>
       </c>
       <c r="E64" s="1">
-        <f t="shared" si="8"/>
-        <v>410.71099999999996</v>
-      </c>
-      <c r="F64" s="1">
-        <v>1</v>
-      </c>
-      <c r="G64" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C65" s="1">
-        <v>3.872404</v>
+        <v>500</v>
       </c>
       <c r="D65" s="3">
-        <v>16.07</v>
+        <v>500</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="8"/>
-        <v>18.480499999999999</v>
-      </c>
-      <c r="F65" s="1">
-        <v>10</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>212</v>
+        <v>500</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G65" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C66" s="1">
-        <v>16.879968999999999</v>
+        <v>240.5</v>
       </c>
       <c r="D66" s="3">
-        <v>19.57</v>
+        <v>358.8</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" si="8"/>
-        <v>22.505499999999998</v>
+        <f t="shared" ref="E66:E76" si="9">+D66*1.15</f>
+        <v>412.62</v>
       </c>
       <c r="F66" s="1">
-        <v>10</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>213</v>
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C67" s="1">
-        <v>36.583019</v>
+        <v>0</v>
       </c>
       <c r="D67" s="3">
-        <v>104.35</v>
+        <v>112.32</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" si="8"/>
-        <v>120.00249999999998</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>210</v>
+        <f t="shared" si="9"/>
+        <v>129.16799999999998</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
       </c>
       <c r="G67" s="1" t="b">
         <v>1</v>
@@ -2929,23 +2933,23 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C68" s="1">
-        <v>56.479194999999997</v>
+        <v>4</v>
       </c>
       <c r="D68" s="3">
-        <v>140.18</v>
+        <v>16</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="8"/>
-        <v>161.20699999999999</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>207</v>
+        <f t="shared" si="9"/>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
       </c>
       <c r="G68" s="1" t="b">
         <v>1</v>
@@ -2955,22 +2959,23 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C69" s="1">
-        <v>500</v>
+        <v>13.5</v>
       </c>
       <c r="D69" s="3">
-        <v>500</v>
+        <v>16.559999999999999</v>
       </c>
       <c r="E69" s="1">
-        <v>300</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>2</v>
+        <f t="shared" si="9"/>
+        <v>19.043999999999997</v>
+      </c>
+      <c r="F69" s="1">
+        <v>4</v>
       </c>
       <c r="G69" s="1" t="b">
         <v>1</v>
@@ -2980,23 +2985,23 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C70" s="1">
-        <v>240.5</v>
+        <v>5.89</v>
       </c>
       <c r="D70" s="3">
-        <v>358.8</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" ref="E70:E81" si="9">+D70*1.15</f>
-        <v>412.62</v>
+        <f t="shared" si="9"/>
+        <v>9.5219999999999985</v>
       </c>
       <c r="F70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G70" s="1" t="b">
         <v>1</v>
@@ -3006,20 +3011,20 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C71" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D71" s="3">
-        <v>112.32</v>
+        <v>134.78</v>
       </c>
       <c r="E71" s="1">
         <f t="shared" si="9"/>
-        <v>129.16799999999998</v>
+        <v>154.99699999999999</v>
       </c>
       <c r="F71" s="1">
         <v>1</v>
@@ -3032,23 +3037,23 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C72" s="1">
-        <v>4</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="D72" s="3">
-        <v>16</v>
+        <v>21.74</v>
       </c>
       <c r="E72" s="1">
         <f t="shared" si="9"/>
-        <v>18.399999999999999</v>
+        <v>25.000999999999998</v>
       </c>
       <c r="F72" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G72" s="1" t="b">
         <v>1</v>
@@ -3058,23 +3063,23 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C73" s="1">
-        <v>13.5</v>
+        <v>3.55</v>
       </c>
       <c r="D73" s="3">
-        <v>16.559999999999999</v>
+        <v>8.48</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" si="9"/>
-        <v>19.043999999999997</v>
-      </c>
-      <c r="F73" s="1">
-        <v>4</v>
+        <v>9.7519999999999989</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="G73" s="1" t="b">
         <v>1</v>
@@ -3084,23 +3089,23 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>121</v>
+        <v>199</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="C74" s="1">
-        <v>5.89</v>
+        <v>0.5</v>
       </c>
       <c r="D74" s="3">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="E74" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E74" s="6">
         <f t="shared" si="9"/>
-        <v>9.5219999999999985</v>
-      </c>
-      <c r="F74" s="1">
-        <v>2</v>
+        <v>2.875</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="G74" s="1" t="b">
         <v>1</v>
@@ -3110,28 +3115,27 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C75" s="1">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D75" s="3">
-        <v>134.78</v>
+        <v>80</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" si="9"/>
-        <v>154.99699999999999</v>
-      </c>
-      <c r="F75" s="1">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="G75" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3142,17 +3146,17 @@
         <v>138</v>
       </c>
       <c r="C76" s="1">
-        <v>8.7100000000000009</v>
+        <v>3.5</v>
       </c>
       <c r="D76" s="3">
-        <v>21.74</v>
+        <v>6</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" si="9"/>
-        <v>25.000999999999998</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="F76" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G76" s="1" t="b">
         <v>1</v>
@@ -3161,131 +3165,43 @@
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C77" s="1">
-        <v>3.55</v>
-      </c>
-      <c r="D77" s="3">
-        <v>8.48</v>
-      </c>
-      <c r="E77" s="1">
-        <f t="shared" si="9"/>
-        <v>9.7519999999999989</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G77" s="1" t="b">
+      <c r="A77" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C77" s="6">
+        <v>250</v>
+      </c>
+      <c r="D77" s="10">
+        <v>250</v>
+      </c>
+      <c r="E77" s="6">
+        <v>250</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G77" s="6" t="b">
         <v>1</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C78" s="1">
-        <v>61.337499999999999</v>
-      </c>
-      <c r="D78" s="3">
-        <v>252.17</v>
-      </c>
-      <c r="E78" s="1">
-        <f t="shared" si="9"/>
-        <v>289.99549999999994</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G78" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C79" s="1">
-        <v>80</v>
-      </c>
-      <c r="D79" s="3">
-        <v>80</v>
-      </c>
-      <c r="E79" s="1">
-        <f t="shared" si="9"/>
-        <v>92</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G79" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C80" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="D80" s="3">
-        <v>6</v>
-      </c>
-      <c r="E80" s="1">
-        <f t="shared" si="9"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="F80" s="1">
-        <v>1</v>
-      </c>
-      <c r="G80" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C81" s="6">
-        <v>800</v>
-      </c>
-      <c r="D81" s="10">
-        <v>1500</v>
-      </c>
-      <c r="E81" s="6">
-        <f t="shared" si="9"/>
-        <v>1724.9999999999998</v>
-      </c>
-      <c r="F81" s="6">
-        <v>1</v>
-      </c>
-      <c r="G81" s="6" t="b">
-        <v>1</v>
-      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
@@ -3322,6 +3238,13 @@
       <c r="I89" s="1"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
@@ -3330,27 +3253,13 @@
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Update in excel data_base
</commit_message>
<xml_diff>
--- a/Elevators.xlsx
+++ b/Elevators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Desktop/Invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AF4DF7-728D-A047-85DA-EEEDDB29825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72C70A5-69D9-4746-B37C-2F40681787B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
   </bookViews>
   <sheets>
     <sheet name="PartsRules" sheetId="3" r:id="rId1"/>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B74E1E-2FAB-A84A-BD4C-ED601BD34DA2}">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="98" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2507,7 +2507,7 @@
         <v>1794</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" ref="E51:E64" si="8">+D51*1.15</f>
+        <f t="shared" ref="E51:E63" si="8">+D51*1.15</f>
         <v>2063.1</v>
       </c>
       <c r="F51" s="1" t="s">

</xml_diff>

<commit_message>
Update the code and data base
</commit_message>
<xml_diff>
--- a/Elevators.xlsx
+++ b/Elevators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Desktop/Invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFA8AAA-DAC5-2146-B499-2F03D39C5024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58908514-A5A0-494B-9E1B-34B3518E51A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2B9F029B-6AF5-494F-B4F8-F754E85C0FC6}"/>
   </bookViews>
@@ -711,7 +711,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1192,11 +1192,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B74E1E-2FAB-A84A-BD4C-ED601BD34DA2}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="88" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="101.1640625" customWidth="1"/>
@@ -1208,7 +1208,7 @@
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>15</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>109</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>197</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>199</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>200</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>201</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>111</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>192</v>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>113</v>
       </c>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>114</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>164</v>
       </c>
       <c r="C21" s="22">
-        <v>963.69500000000005</v>
+        <v>1190</v>
       </c>
       <c r="D21" s="22">
         <v>2869.57</v>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>129</v>
       </c>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>129</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -1907,7 +1907,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>115</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1987,7 +1987,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2088,7 +2088,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -2114,7 +2114,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -2270,7 +2270,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>168</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2452,7 +2452,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -2608,7 +2608,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>61</v>
       </c>
@@ -2634,7 +2634,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -2660,7 +2660,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -2712,7 +2712,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>69</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
@@ -2764,7 +2764,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>77</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>79</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
@@ -2842,7 +2842,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>83</v>
       </c>
@@ -2868,7 +2868,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>87</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>89</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>91</v>
       </c>
@@ -2972,7 +2972,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>93</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>176</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>95</v>
       </c>
@@ -3048,7 +3048,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>97</v>
       </c>
@@ -3074,7 +3074,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
@@ -3100,7 +3100,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>102</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>104</v>
       </c>
@@ -3152,7 +3152,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>106</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>117</v>
       </c>
@@ -3204,7 +3204,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>119</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>171</v>
       </c>
@@ -3256,7 +3256,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>121</v>
       </c>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>125</v>
       </c>
@@ -3307,7 +3307,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>167</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
         <v>189</v>
       </c>
@@ -3358,57 +3358,57 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>206</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>207</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3419,20 +3419,20 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="9:9">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I97" s="1"/>
     </row>
   </sheetData>

</xml_diff>